<commit_message>
Update: PCM2704 HPA ブロック図.xlsx
</commit_message>
<xml_diff>
--- a/PCM2704 HPA ブロック図.xlsx
+++ b/PCM2704 HPA ブロック図.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Users\nerdfloor\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Users\nerdfloor\Documents\Develop\PCM2704_HPA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{635F7A10-FC6E-42CF-A0E9-828F29AFDCD2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{735F1A9E-7C90-43C3-967D-043A62FBE772}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="585" yWindow="600" windowWidth="21990" windowHeight="13830" xr2:uid="{4917A1BD-E6FD-4AFD-AC47-A93828C35F47}"/>
+    <workbookView xWindow="585" yWindow="600" windowWidth="16920" windowHeight="14940" xr2:uid="{4917A1BD-E6FD-4AFD-AC47-A93828C35F47}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -68,13 +68,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>※1 バイパス可能とする。</t>
-    <rPh sb="7" eb="9">
-      <t>カノウ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>デジタル系</t>
     <rPh sb="4" eb="5">
       <t>ケイ</t>
@@ -95,12 +88,22 @@
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
+  <si>
+    <t>※1 LME49600のHPFは無効化可能。</t>
+    <rPh sb="16" eb="19">
+      <t>ムコウカ</t>
+    </rPh>
+    <rPh sb="19" eb="21">
+      <t>カノウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -113,6 +116,15 @@
       <sz val="6"/>
       <name val="游ゴシック"/>
       <family val="2"/>
+      <charset val="128"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="游ゴシック"/>
+      <family val="3"/>
       <charset val="128"/>
       <scheme val="minor"/>
     </font>
@@ -139,8 +151,11 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -427,13 +442,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
+      <xdr:col>16</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>15</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
+      <xdr:col>20</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>21</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -451,7 +466,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2667000" y="2476500"/>
+          <a:off x="3048000" y="2857500"/>
           <a:ext cx="762000" cy="1143000"/>
         </a:xfrm>
         <a:prstGeom prst="homePlate">
@@ -673,14 +688,14 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -695,7 +710,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1152525" y="2857500"/>
+          <a:off x="390525" y="3800475"/>
           <a:ext cx="381000" cy="381000"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
@@ -732,14 +747,14 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>18</xdr:row>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>21</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -755,8 +770,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1524000" y="3048000"/>
-          <a:ext cx="381000" cy="0"/>
+          <a:off x="771525" y="4000500"/>
+          <a:ext cx="561975" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -784,13 +799,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
+      <xdr:col>12</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>15</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
+      <xdr:col>16</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>21</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -808,7 +823,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1905000" y="2476500"/>
+          <a:off x="2286000" y="2857500"/>
           <a:ext cx="762000" cy="1143000"/>
         </a:xfrm>
         <a:prstGeom prst="homePlate">
@@ -848,7 +863,7 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>14</xdr:col>
+      <xdr:col>20</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>18</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -868,12 +883,14 @@
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
+        <xdr:cNvCxnSpPr>
+          <a:endCxn id="10" idx="2"/>
+        </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3429000" y="3048000"/>
-          <a:ext cx="2476500" cy="0"/>
+          <a:off x="3810000" y="3429000"/>
+          <a:ext cx="571500" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -1015,14 +1032,14 @@
     <xdr:from>
       <xdr:col>47</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>190499</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>49</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>190499</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1037,7 +1054,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10096500" y="4762500"/>
+          <a:off x="8953500" y="4952999"/>
           <a:ext cx="381000" cy="381000"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
@@ -1511,14 +1528,14 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>9524</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>46</xdr:col>
       <xdr:colOff>190499</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>190499</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -1536,8 +1553,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm rot="16200000" flipH="1">
-          <a:off x="4386262" y="-185738"/>
-          <a:ext cx="762000" cy="8372475"/>
+          <a:off x="4286250" y="476249"/>
+          <a:ext cx="962024" cy="8372475"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector2">
           <a:avLst/>
@@ -1913,13 +1930,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>27</xdr:row>
+      <xdr:row>30</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>28</xdr:row>
+      <xdr:row>31</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1973,13 +1990,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>28</xdr:row>
+      <xdr:row>31</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>29</xdr:row>
+      <xdr:row>32</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2033,13 +2050,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>29</xdr:row>
+      <xdr:row>32</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>30</xdr:row>
+      <xdr:row>33</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2092,9 +2109,9 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>21</xdr:col>
-      <xdr:colOff>38100</xdr:colOff>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>23</xdr:col>
@@ -2117,12 +2134,429 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1" flipV="1">
-          <a:off x="4038600" y="2295525"/>
-          <a:ext cx="342900" cy="371475"/>
+          <a:off x="4000500" y="2286000"/>
+          <a:ext cx="381000" cy="381000"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
         </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="35" name="楕円 34">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F8468024-4911-45CE-BE7E-C140B4D62453}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1333500" y="3238500"/>
+          <a:ext cx="381000" cy="381000"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent2">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>180974</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>180974</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="38" name="楕円 37">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A3D4C698-7E78-42BA-B7C0-B11C22EDDBF5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1333500" y="3800474"/>
+          <a:ext cx="381000" cy="381000"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent2">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>190499</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>190499</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="40" name="正方形/長方形 39">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D90C7E4D-C100-4751-9FCC-FA61F570FF46}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1143000" y="2857499"/>
+          <a:ext cx="762000" cy="2095500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="19050"/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:t>Bypass</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100" baseline="0"/>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:t>SW</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="44" name="楕円 43">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B1EA4244-534F-4E5A-8E21-77038D36D751}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1333500" y="4381500"/>
+          <a:ext cx="381000" cy="381000"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent2">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>190499</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>180974</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="46" name="直線コネクタ 45">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6CF79BCA-9557-402E-8F52-EE54CEE2FB4A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="38" idx="2"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="952500" y="3619499"/>
+          <a:ext cx="381000" cy="371475"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="49" name="直線矢印コネクタ 48">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A05DF59D-1012-410E-A660-08B28B4643E3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="35" idx="6"/>
+          <a:endCxn id="16" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1714500" y="3429000"/>
+          <a:ext cx="571500" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="30" name="コネクタ: カギ線 29">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{28745335-469C-4206-A7A2-2F668800141E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="44" idx="6"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="1714500" y="3429000"/>
+          <a:ext cx="2286000" cy="1143000"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 100000"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
       </xdr:spPr>
       <xdr:style>
         <a:lnRef idx="3">
@@ -2444,16 +2878,16 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B2:AV30"/>
+  <dimension ref="B2:AV33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AN30" sqref="AN30"/>
+      <selection sqref="A1:AZ34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.4"/>
   <sheetData>
     <row r="2" spans="2:48" ht="15" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
@@ -2482,40 +2916,40 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="3:48" ht="15" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C17" t="s">
+    <row r="20" spans="3:48" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="C20" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="3:48" ht="15" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="AV22" t="s">
+    <row r="26" spans="3:48" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="AV26" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="3:48" ht="15" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="D26" t="s">
+    <row r="29" spans="3:48" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="D29" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="31" spans="3:48" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="F31" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="28" spans="3:48" ht="15" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="F28" t="s">
+    <row r="32" spans="3:48" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="F32" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="29" spans="3:48" ht="15" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="F29" t="s">
+    <row r="33" spans="6:6" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="F33" t="s">
         <v>10</v>
-      </c>
-    </row>
-    <row r="30" spans="3:48" ht="15" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="F30" t="s">
-        <v>11</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="91" orientation="landscape" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="94" orientation="landscape" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>